<commit_message>
update volo inventory and germination results
</commit_message>
<xml_diff>
--- a/resources/volo-data/volo-inventory.xlsx
+++ b/resources/volo-data/volo-inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anneliserismann/Documents/GitHub/hdbot/resources/volo-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD484767-6ADC-964F-A63C-3F5B7E8F2446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9280D6-4C0E-5647-88DA-21F028DAECAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9BEEE2E6-61EF-3C4B-9A35-B98E6E0B029E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{9BEEE2E6-61EF-3C4B-9A35-B98E6E0B029E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$G$438</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1205,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2372BBF7-4E74-B647-AFAB-894F6CB11742}">
   <dimension ref="A1:G438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>